<commit_message>
Set percent of fuel demand changes that affect exports to 1
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\Dropbox (Energy InNovation)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E0567-D228-475F-AE92-CB99F12E58B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data from BFPIaE" sheetId="3" r:id="rId2"/>
     <sheet name="PoFDCtAE" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -340,7 +339,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
@@ -787,22 +786,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="87.5703125" customWidth="1"/>
+    <col min="2" max="2" width="87.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -810,223 +809,223 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="32" t="s">
         <v>92</v>
       </c>
       <c r="B47" s="33"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="14" t="s">
         <v>53</v>
       </c>
@@ -1038,87 +1037,87 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1126,26 +1125,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-    <col min="2" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="100.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.1328125" customWidth="1"/>
+    <col min="2" max="5" width="15.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="100.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>70</v>
       </c>
@@ -1158,7 +1157,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="18" t="s">
         <v>71</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1244,7 +1243,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
@@ -1269,7 +1268,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
@@ -1294,7 +1293,7 @@
       <c r="F9" s="23"/>
       <c r="G9" s="30"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
@@ -1305,7 +1304,7 @@
       <c r="F10" s="23"/>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
@@ -1327,7 +1326,7 @@
       </c>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="28" t="s">
         <v>40</v>
       </c>
@@ -1349,7 +1348,7 @@
       </c>
       <c r="G12" s="30"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="28" t="s">
         <v>41</v>
       </c>
@@ -1371,7 +1370,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
@@ -1393,7 +1392,7 @@
       </c>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1414,7 @@
       </c>
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="28" t="s">
         <v>44</v>
       </c>
@@ -1437,7 +1436,7 @@
       </c>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
@@ -1448,7 +1447,7 @@
       <c r="F17" s="23"/>
       <c r="G17" s="30"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -1459,7 +1458,7 @@
       <c r="F18" s="23"/>
       <c r="G18" s="30"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
@@ -1481,7 +1480,7 @@
       </c>
       <c r="G19" s="30"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
@@ -1503,7 +1502,7 @@
       </c>
       <c r="G20" s="30"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="28" t="s">
         <v>49</v>
       </c>
@@ -1525,7 +1524,7 @@
       </c>
       <c r="G21" s="30"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="28" t="s">
         <v>50</v>
       </c>
@@ -1547,7 +1546,7 @@
       </c>
       <c r="G22" s="30"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>51</v>
       </c>
@@ -1569,7 +1568,7 @@
       </c>
       <c r="G23" s="30"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
@@ -1597,7 +1596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1607,16 +1606,16 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="22" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.73046875" customWidth="1"/>
+    <col min="2" max="22" width="16.59765625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>69</v>
       </c>
@@ -1684,7 +1683,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -1752,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1760,8 +1759,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="31">
-        <f>'Data from BFPIaE'!D5/'Data from BFPIaE'!B5</f>
-        <v>0.14686588977933832</v>
+        <v>1</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1821,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1832,8 +1830,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="31">
-        <f>'Data from BFPIaE'!D6/'Data from BFPIaE'!B6</f>
-        <v>0.15500746052469119</v>
+        <v>1</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -1890,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -1959,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -2027,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -2095,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -2163,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -2189,8 +2186,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="31">
-        <f>'Data from BFPIaE'!D11/'Data from BFPIaE'!B11</f>
-        <v>0.68036965837987495</v>
+        <v>1</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -2232,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
@@ -2261,8 +2257,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="12">
-        <f>'Data from BFPIaE'!D12/SUM('Data from BFPIaE'!D12:E12)</f>
-        <v>7.2806513229885905E-2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="8">
         <v>0</v>
@@ -2287,7 +2282,7 @@
       </c>
       <c r="R10" s="13">
         <f>1-J10</f>
-        <v>0.92719348677011415</v>
+        <v>0</v>
       </c>
       <c r="S10" s="8">
         <v>0</v>
@@ -2302,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -2334,8 +2329,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="12">
-        <f>'Data from BFPIaE'!D13/SUM('Data from BFPIaE'!D13:E13)</f>
-        <v>0.26002912808189416</v>
+        <v>1</v>
       </c>
       <c r="L11" s="8">
         <v>0</v>
@@ -2357,7 +2351,7 @@
       </c>
       <c r="R11" s="13">
         <f>1-K11</f>
-        <v>0.73997087191810584</v>
+        <v>0</v>
       </c>
       <c r="S11" s="8">
         <v>0</v>
@@ -2372,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -2407,8 +2401,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="31">
-        <f>'Data from BFPIaE'!D14/'Data from BFPIaE'!B14</f>
-        <v>0.10491259896601664</v>
+        <v>1</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -2441,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
@@ -2479,8 +2472,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="31">
-        <f>'Data from BFPIaE'!D15/'Data from BFPIaE'!B15</f>
-        <v>7.0542950086431883E-2</v>
+        <v>1</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -2510,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
@@ -2551,8 +2543,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="12">
-        <f>'Data from BFPIaE'!D16/SUM('Data from BFPIaE'!D16:E16)</f>
-        <v>9.9755024140854479E-2</v>
+        <v>1</v>
       </c>
       <c r="O14" s="11">
         <v>0</v>
@@ -2565,7 +2556,7 @@
       </c>
       <c r="R14" s="13">
         <f>1-N14</f>
-        <v>0.90024497585914554</v>
+        <v>0</v>
       </c>
       <c r="S14" s="8">
         <v>0</v>
@@ -2580,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
@@ -2648,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -2716,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -2785,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
@@ -2853,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -2907,11 +2898,10 @@
       </c>
       <c r="R19" s="13">
         <f>1-S19</f>
-        <v>0.49404181432894001</v>
+        <v>0</v>
       </c>
       <c r="S19" s="12">
-        <f>'Data from BFPIaE'!D21/SUM('Data from BFPIaE'!D21:E21)</f>
-        <v>0.50595818567105999</v>
+        <v>1</v>
       </c>
       <c r="T19" s="8">
         <v>0</v>
@@ -2923,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
@@ -2977,14 +2967,13 @@
       </c>
       <c r="R20" s="13">
         <f>1-T20</f>
-        <v>0.57774176716224113</v>
+        <v>0</v>
       </c>
       <c r="S20" s="8">
         <v>0</v>
       </c>
       <c r="T20" s="12">
-        <f>'Data from BFPIaE'!D22/SUM('Data from BFPIaE'!D22:E22)</f>
-        <v>0.42225823283775882</v>
+        <v>1</v>
       </c>
       <c r="U20" s="8">
         <v>0</v>
@@ -2993,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
@@ -3062,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>

</xml_diff>